<commit_message>
Updated broken links validation code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/inputData.xlsx
+++ b/src/test/resources/TestData/inputData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\train\Automation\HS_Cucumber-main\HomeserveUSA\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\BAU_Regression\BAU_Regression\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D41E868-C9F3-479F-B8CF-8AB75A4AE874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A75C6C-E615-456F-9DC8-52A068C07BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4BD471F-CC96-4C0B-AADD-EAF5A4C4939D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23100" windowHeight="11388" activeTab="1" xr2:uid="{C4BD471F-CC96-4C0B-AADD-EAF5A4C4939D}"/>
   </bookViews>
   <sheets>
     <sheet name="inputData" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">inputData!$A$1:$T$49</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">URL!$A$1:$B$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">URL!$A$1:$B$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="208">
   <si>
     <t>Test ID</t>
   </si>
@@ -650,6 +650,21 @@
   </si>
   <si>
     <t>Paperless</t>
+  </si>
+  <si>
+    <t>HomeserveHome</t>
+  </si>
+  <si>
+    <t>https://www.reghomeserve.com/en-us/?ncr=true</t>
+  </si>
+  <si>
+    <t>TC_SANITY_001</t>
+  </si>
+  <si>
+    <t>Validate all the links in homepage to check for broken links</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -746,7 +761,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -834,12 +849,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -867,6 +906,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1202,11 +1247,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFA7E03-C988-479B-B08E-B46A33901233}">
-  <dimension ref="A1:U49"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F22" sqref="F22"/>
+      <selection pane="topRight" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3782,77 +3827,77 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2" t="s">
+      <c r="C47" s="21"/>
+      <c r="D47" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="F47" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="G47" s="8" t="s">
+      <c r="F47" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="G47" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H47" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="I47" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="J47" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="M47" s="4" t="s">
+      <c r="K47" s="22"/>
+      <c r="L47" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="M47" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="N47" s="8" t="s">
+      <c r="N47" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="O47" s="8" t="s">
+      <c r="O47" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="P47" s="8" t="s">
+      <c r="P47" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="Q47" s="8" t="s">
+      <c r="Q47" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="R47" s="5" t="s">
+      <c r="R47" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="S47" s="5" t="s">
+      <c r="S47" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="T47" s="19" t="s">
+      <c r="T47" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="U47" s="5" t="s">
+      <c r="U47" s="25" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C48" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>101</v>
       </c>
       <c r="E48" s="4" t="s">
@@ -3864,7 +3909,7 @@
       <c r="G48" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" s="4" t="s">
         <v>105</v>
       </c>
       <c r="I48" s="4" t="s">
@@ -3906,16 +3951,16 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="C49" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>104</v>
       </c>
       <c r="E49" s="4" t="s">
@@ -3927,7 +3972,7 @@
       <c r="G49" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="H49" s="3" t="s">
+      <c r="H49" s="4" t="s">
         <v>105</v>
       </c>
       <c r="I49" s="4" t="s">
@@ -3966,6 +4011,71 @@
       </c>
       <c r="U49" s="5" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="P50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="S50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="T50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="U50" s="4" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3977,10 +4087,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F731B1-F395-44C8-A5FA-27912FB095EB}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4013,90 +4123,90 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>175</v>
+        <v>203</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>204</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>137</v>
+        <v>14</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>175</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>124</v>
+        <v>137</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>125</v>
+        <v>34</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>127</v>
+        <v>141</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>128</v>
+        <v>176</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -4107,231 +4217,243 @@
         <v>142</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B15" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B16" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="11" t="s">
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B18" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="11" t="s">
-        <v>150</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="11" t="s">
         <v>154</v>
-      </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>155</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B27" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
-      <c r="B30" s="10" t="s">
-        <v>139</v>
+      <c r="B30" s="11" t="s">
+        <v>162</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="10" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
-      <c r="B33" s="14" t="s">
-        <v>163</v>
+      <c r="B33" s="10" t="s">
+        <v>159</v>
       </c>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
+      <c r="B35" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="C34" s="5"/>
+      <c r="C35" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B34" xr:uid="{74F731B1-F395-44C8-A5FA-27912FB095EB}"/>
+  <autoFilter ref="A1:B35" xr:uid="{74F731B1-F395-44C8-A5FA-27912FB095EB}"/>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{74ABD3DF-CF3D-42EA-9CFF-86C14D400C7B}"/>
-    <hyperlink ref="B14" r:id="rId2" display="https://www.reghomeserve.com/sc/mail/firstenergy-fundle" xr:uid="{AD8FB8C2-15C4-4D6F-A210-EF42DC585205}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{23C72C45-07E2-4339-8161-4D4A291A3480}"/>
-    <hyperlink ref="B8" r:id="rId4" display="https://preprod.slwofa.com/mail/lasanitation" xr:uid="{01FF8113-D8EB-48D2-9B71-50BBBCA61BA5}"/>
-    <hyperlink ref="B9" r:id="rId5" display="https://www.reghomeserve.com/sc/mail/buffalowaternipcnew" xr:uid="{9C4F3023-4BB6-4851-ADF7-BB0B9087D372}"/>
-    <hyperlink ref="B6" location="MTW_NIPC!A1" display="MTW_NIPC!A1" xr:uid="{94A2B24C-DFA3-4864-A388-C2FE67D2B4A0}"/>
-    <hyperlink ref="B10" location="MTW_Regular!A1" display="MTW_Regular!A1" xr:uid="{6FD6BC41-D7C9-4F6C-8F60-C2C3CA14A0F8}"/>
-    <hyperlink ref="B11" location="MTW_Regular!A1" display="MTW_Regular!A1" xr:uid="{8AD7AB3A-74C5-4A98-8C18-13EE5049A030}"/>
-    <hyperlink ref="B4" location="SLWA!A1" display="SLWA!A1" xr:uid="{907FA7E2-AC6B-4595-A31F-343F62B96378}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{D51DB6C3-7C46-47CB-AB8C-D1E1F0CB4FE2}"/>
-    <hyperlink ref="B5" location="SLWC!A1" display="SLWC!A1" xr:uid="{934C7837-F3F5-4735-AD16-72E13190A180}"/>
-    <hyperlink ref="B15" r:id="rId7" xr:uid="{993C9669-F345-4AA6-93CA-F34C7AC1CF73}"/>
-    <hyperlink ref="B16" r:id="rId8" xr:uid="{42F57244-0C52-4995-ADB3-9C89BD1BD6B7}"/>
-    <hyperlink ref="B17" r:id="rId9" xr:uid="{F11D9593-6C33-4EC4-B906-83FF61C41959}"/>
-    <hyperlink ref="B18" location="Landing_Pages!A1" display="Landing_Pages!A1" xr:uid="{3BF5AD64-D6C9-45DE-A3DB-73538B41055D}"/>
-    <hyperlink ref="B19" r:id="rId10" xr:uid="{89D1732F-95A1-4909-B2A4-E1F6924D670D}"/>
-    <hyperlink ref="B20" location="Landing_Pages!A1" display="Landing_Pages!A1" xr:uid="{E3FFBD4A-6299-48BC-AE41-CE5A2AC77EAD}"/>
-    <hyperlink ref="B21" r:id="rId11" xr:uid="{B524328F-D2BC-43F7-9336-22C4D13E6231}"/>
-    <hyperlink ref="B22" r:id="rId12" xr:uid="{AB16D659-A07A-46E4-B570-71BBDA57EDAA}"/>
-    <hyperlink ref="B23" r:id="rId13" xr:uid="{00EDA3E7-F7F9-447C-9E55-43030810D1EE}"/>
-    <hyperlink ref="B24" location="STS_CNPEE!A1" display="STS_CNPEE!A1" xr:uid="{1BA1C733-89E6-481F-B709-368006107BC6}"/>
-    <hyperlink ref="B25" location="STS_CNPEG!A1" display="STS_CNPEG!A1" xr:uid="{7366C463-7134-41C2-8817-9495FC636056}"/>
-    <hyperlink ref="B26" location="Techupsell-Albama!A1" display="Techupsell-Albama!A1" xr:uid="{5C84A0D3-3570-4CE7-B77A-EA4D516C113F}"/>
-    <hyperlink ref="B27" location="Tech_App!A1" display="Tech_App!A1" xr:uid="{20507C38-686C-4071-A626-2D67B41CD89A}"/>
-    <hyperlink ref="B28" location="Techupsell!A1" display="Techupsell!A1" xr:uid="{331BB979-42ED-448F-BF85-450E5550FC3F}"/>
-    <hyperlink ref="B29" location="Techupsell_FPL!A1" display="Techupsell_FPL!A1" xr:uid="{E35CA4BE-F1AD-411F-B3EC-2AC78D25A613}"/>
-    <hyperlink ref="B30" location="CCPA!A1" display="CCPA!A1" xr:uid="{D439AEA1-F8C0-4FA7-9E10-E90D5D3DADF8}"/>
-    <hyperlink ref="B31" location="CCPA!A1" display="CCPA!A1" xr:uid="{DF9404B4-5150-4CD4-9C75-28A9558DE473}"/>
-    <hyperlink ref="B32" r:id="rId14" display="https://www.reghomeserve.com/us/whqe" xr:uid="{4A56A19F-CDE8-48DE-ACA9-F3E5DA0D73C4}"/>
-    <hyperlink ref="B33" location="Partner Portal!A1" display="Partner Portal!A1" xr:uid="{F609080B-E38C-4402-A9B0-E7E7001B14BD}"/>
-    <hyperlink ref="B3" r:id="rId15" xr:uid="{314A0927-1471-4219-9F92-31597DD504FD}"/>
-    <hyperlink ref="B12" r:id="rId16" xr:uid="{8EB57EB5-EE83-42C2-B0BB-CE85AEF20287}"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{74ABD3DF-CF3D-42EA-9CFF-86C14D400C7B}"/>
+    <hyperlink ref="B15" r:id="rId2" display="https://www.reghomeserve.com/sc/mail/firstenergy-fundle" xr:uid="{AD8FB8C2-15C4-4D6F-A210-EF42DC585205}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{23C72C45-07E2-4339-8161-4D4A291A3480}"/>
+    <hyperlink ref="B9" r:id="rId4" display="https://preprod.slwofa.com/mail/lasanitation" xr:uid="{01FF8113-D8EB-48D2-9B71-50BBBCA61BA5}"/>
+    <hyperlink ref="B10" r:id="rId5" display="https://www.reghomeserve.com/sc/mail/buffalowaternipcnew" xr:uid="{9C4F3023-4BB6-4851-ADF7-BB0B9087D372}"/>
+    <hyperlink ref="B7" location="MTW_NIPC!A1" display="MTW_NIPC!A1" xr:uid="{94A2B24C-DFA3-4864-A388-C2FE67D2B4A0}"/>
+    <hyperlink ref="B11" location="MTW_Regular!A1" display="MTW_Regular!A1" xr:uid="{6FD6BC41-D7C9-4F6C-8F60-C2C3CA14A0F8}"/>
+    <hyperlink ref="B12" location="MTW_Regular!A1" display="MTW_Regular!A1" xr:uid="{8AD7AB3A-74C5-4A98-8C18-13EE5049A030}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{907FA7E2-AC6B-4595-A31F-343F62B96378}"/>
+    <hyperlink ref="B2" r:id="rId7" xr:uid="{D51DB6C3-7C46-47CB-AB8C-D1E1F0CB4FE2}"/>
+    <hyperlink ref="B6" location="SLWC!A1" display="SLWC!A1" xr:uid="{934C7837-F3F5-4735-AD16-72E13190A180}"/>
+    <hyperlink ref="B16" r:id="rId8" xr:uid="{993C9669-F345-4AA6-93CA-F34C7AC1CF73}"/>
+    <hyperlink ref="B17" r:id="rId9" xr:uid="{42F57244-0C52-4995-ADB3-9C89BD1BD6B7}"/>
+    <hyperlink ref="B18" r:id="rId10" xr:uid="{F11D9593-6C33-4EC4-B906-83FF61C41959}"/>
+    <hyperlink ref="B19" location="Landing_Pages!A1" display="Landing_Pages!A1" xr:uid="{3BF5AD64-D6C9-45DE-A3DB-73538B41055D}"/>
+    <hyperlink ref="B20" r:id="rId11" xr:uid="{89D1732F-95A1-4909-B2A4-E1F6924D670D}"/>
+    <hyperlink ref="B21" location="Landing_Pages!A1" display="Landing_Pages!A1" xr:uid="{E3FFBD4A-6299-48BC-AE41-CE5A2AC77EAD}"/>
+    <hyperlink ref="B22" r:id="rId12" xr:uid="{B524328F-D2BC-43F7-9336-22C4D13E6231}"/>
+    <hyperlink ref="B23" r:id="rId13" xr:uid="{AB16D659-A07A-46E4-B570-71BBDA57EDAA}"/>
+    <hyperlink ref="B24" r:id="rId14" xr:uid="{00EDA3E7-F7F9-447C-9E55-43030810D1EE}"/>
+    <hyperlink ref="B25" location="STS_CNPEE!A1" display="STS_CNPEE!A1" xr:uid="{1BA1C733-89E6-481F-B709-368006107BC6}"/>
+    <hyperlink ref="B26" location="STS_CNPEG!A1" display="STS_CNPEG!A1" xr:uid="{7366C463-7134-41C2-8817-9495FC636056}"/>
+    <hyperlink ref="B27" location="Techupsell-Albama!A1" display="Techupsell-Albama!A1" xr:uid="{5C84A0D3-3570-4CE7-B77A-EA4D516C113F}"/>
+    <hyperlink ref="B28" location="Tech_App!A1" display="Tech_App!A1" xr:uid="{20507C38-686C-4071-A626-2D67B41CD89A}"/>
+    <hyperlink ref="B29" location="Techupsell!A1" display="Techupsell!A1" xr:uid="{331BB979-42ED-448F-BF85-450E5550FC3F}"/>
+    <hyperlink ref="B30" location="Techupsell_FPL!A1" display="Techupsell_FPL!A1" xr:uid="{E35CA4BE-F1AD-411F-B3EC-2AC78D25A613}"/>
+    <hyperlink ref="B31" location="CCPA!A1" display="CCPA!A1" xr:uid="{D439AEA1-F8C0-4FA7-9E10-E90D5D3DADF8}"/>
+    <hyperlink ref="B32" location="CCPA!A1" display="CCPA!A1" xr:uid="{DF9404B4-5150-4CD4-9C75-28A9558DE473}"/>
+    <hyperlink ref="B33" r:id="rId15" display="https://www.reghomeserve.com/us/whqe" xr:uid="{4A56A19F-CDE8-48DE-ACA9-F3E5DA0D73C4}"/>
+    <hyperlink ref="B34" location="Partner Portal!A1" display="Partner Portal!A1" xr:uid="{F609080B-E38C-4402-A9B0-E7E7001B14BD}"/>
+    <hyperlink ref="B4" r:id="rId16" xr:uid="{314A0927-1471-4219-9F92-31597DD504FD}"/>
+    <hyperlink ref="B13" r:id="rId17" xr:uid="{8EB57EB5-EE83-42C2-B0BB-CE85AEF20287}"/>
+    <hyperlink ref="B3" r:id="rId18" xr:uid="{17500D8F-EF7E-4F10-BA1D-AB299ECD5413}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Kandela test script
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/inputData.xlsx
+++ b/src/test/resources/TestData/inputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\BAU_Regression\BAU_Regression\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A75C6C-E615-456F-9DC8-52A068C07BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963DB359-D558-43C1-BF00-7845CAB069DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23100" windowHeight="11388" activeTab="1" xr2:uid="{C4BD471F-CC96-4C0B-AADD-EAF5A4C4939D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23100" windowHeight="11388" xr2:uid="{C4BD471F-CC96-4C0B-AADD-EAF5A4C4939D}"/>
   </bookViews>
   <sheets>
     <sheet name="inputData" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="211">
   <si>
     <t>Test ID</t>
   </si>
@@ -665,6 +665,15 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>TC_049</t>
+  </si>
+  <si>
+    <t>Complete a sale in HomeServe kandela</t>
+  </si>
+  <si>
+    <t>19146</t>
   </si>
 </sst>
 </file>
@@ -761,7 +770,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -873,12 +882,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -912,6 +939,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1247,11 +1279,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFA7E03-C988-479B-B08E-B46A33901233}">
-  <dimension ref="A1:U50"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D60" sqref="D60"/>
+      <selection pane="topRight" activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4032,50 +4064,113 @@
       <c r="F50" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="G50" s="4" t="s">
+      <c r="G50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="H50" s="4" t="s">
+      <c r="H50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="I50" s="4" t="s">
+      <c r="I50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="J50" s="4" t="s">
+      <c r="J50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="K50" s="4" t="s">
+      <c r="K50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="L50" s="4" t="s">
+      <c r="L50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="M50" s="4" t="s">
+      <c r="M50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="N50" s="4" t="s">
+      <c r="N50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="O50" s="4" t="s">
+      <c r="O50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="P50" s="4" t="s">
+      <c r="P50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="Q50" s="4" t="s">
+      <c r="Q50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="R50" s="4" t="s">
+      <c r="R50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="S50" s="4" t="s">
+      <c r="S50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="T50" s="4" t="s">
+      <c r="T50" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="U50" s="4" t="s">
+      <c r="U50" s="31" t="s">
         <v>207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A51" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="F51" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="N51" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="O51" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="P51" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q51" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="R51" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="S51" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="T51" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="U51" s="5" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -4089,8 +4184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F731B1-F395-44C8-A5FA-27912FB095EB}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated all sanity test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/inputData.xlsx
+++ b/src/test/resources/TestData/inputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\train\Automation\BAU\BAU_Regression\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7061A041-BC39-41E4-AB16-025ED75B36B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C23A94-2CA1-4CA5-A4B0-95DE8021441F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C4BD471F-CC96-4C0B-AADD-EAF5A4C4939D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4BD471F-CC96-4C0B-AADD-EAF5A4C4939D}"/>
   </bookViews>
   <sheets>
     <sheet name="inputData" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="336">
   <si>
     <t>Test ID</t>
   </si>
@@ -796,9 +796,6 @@
     <t>37421</t>
   </si>
   <si>
-    <t>5447558399986310</t>
-  </si>
-  <si>
     <t>VDI</t>
   </si>
   <si>
@@ -1045,13 +1042,13 @@
     <t>https://preprod.slwofc.ca/mail/ottawa</t>
   </si>
   <si>
-    <t>4524007136972670</t>
-  </si>
-  <si>
     <t>https://www.reghomeserve.com/en-us/lp/servline-water/?ncr=true</t>
   </si>
   <si>
     <t>https://www.reghomeserve.com/en-us/clp/display/pk-yellow-no-redirect/?ncr=true</t>
+  </si>
+  <si>
+    <t>Bovonto Street</t>
   </si>
 </sst>
 </file>
@@ -1669,11 +1666,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFA7E03-C988-479B-B08E-B46A33901233}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:Y65"/>
+  <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N56" sqref="N56"/>
+      <selection pane="bottomLeft" activeCell="Q60" sqref="Q60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1682,9 +1679,11 @@
     <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="71.44140625" customWidth="1"/>
-    <col min="5" max="19" width="15.5546875" customWidth="1"/>
+    <col min="5" max="16" width="15.5546875" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="15.5546875" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -1710,7 +1709,7 @@
         <v>112</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I1" s="27" t="s">
         <v>113</v>
@@ -1734,7 +1733,7 @@
         <v>120</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>175</v>
@@ -1800,7 +1799,7 @@
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>181</v>
@@ -1950,9 +1949,7 @@
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1988,10 +1985,10 @@
         <v>190</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>190</v>
@@ -2009,7 +2006,7 @@
         <v>172</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -2054,7 +2051,7 @@
       </c>
       <c r="P6" s="8"/>
       <c r="Q6" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>190</v>
@@ -2072,7 +2069,7 @@
         <v>172</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -2117,7 +2114,7 @@
       </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>190</v>
@@ -2135,7 +2132,7 @@
         <v>172</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
@@ -2145,9 +2142,7 @@
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
@@ -2158,7 +2153,7 @@
         <v>171</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>190</v>
@@ -2170,14 +2165,14 @@
         <v>109</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
         <v>159</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>163</v>
@@ -2201,10 +2196,10 @@
         <v>166</v>
       </c>
       <c r="V8" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="W8" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="W8" s="5" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -2225,7 +2220,7 @@
         <v>171</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="3" t="s">
@@ -2235,14 +2230,14 @@
         <v>109</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4" t="s">
         <v>159</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>163</v>
@@ -2264,10 +2259,10 @@
         <v>166</v>
       </c>
       <c r="V9" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="W9" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="W9" s="5" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -2288,7 +2283,7 @@
         <v>171</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="3" t="s">
@@ -2298,14 +2293,14 @@
         <v>109</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4" t="s">
         <v>159</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O10" s="8" t="s">
         <v>163</v>
@@ -2327,10 +2322,10 @@
         <v>166</v>
       </c>
       <c r="V10" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="W10" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="W10" s="5" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
@@ -2340,9 +2335,7 @@
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
@@ -2378,7 +2371,7 @@
         <v>190</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q11" s="8" t="s">
         <v>215</v>
@@ -2396,10 +2389,10 @@
         <v>166</v>
       </c>
       <c r="V11" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="W11" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="W11" s="5" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -2459,10 +2452,10 @@
         <v>166</v>
       </c>
       <c r="V12" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="W12" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="W12" s="5" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -2522,10 +2515,10 @@
         <v>166</v>
       </c>
       <c r="V13" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="W13" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="W13" s="5" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
@@ -2535,9 +2528,7 @@
       <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
         <v>28</v>
       </c>
@@ -2567,7 +2558,7 @@
         <v>159</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O14" s="8" t="s">
         <v>206</v>
@@ -2591,10 +2582,10 @@
         <v>166</v>
       </c>
       <c r="V14" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="W14" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="W14" s="5" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -2632,7 +2623,7 @@
         <v>159</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O15" s="8" t="s">
         <v>206</v>
@@ -2654,10 +2645,10 @@
         <v>166</v>
       </c>
       <c r="V15" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="W15" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="W15" s="5" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -2695,7 +2686,7 @@
         <v>159</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O16" s="8" t="s">
         <v>206</v>
@@ -2717,10 +2708,10 @@
         <v>166</v>
       </c>
       <c r="V16" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="W16" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="W16" s="5" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
@@ -2730,9 +2721,7 @@
       <c r="B17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>35</v>
       </c>
@@ -2768,10 +2757,10 @@
         <v>190</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R17" s="8" t="s">
         <v>190</v>
@@ -2786,10 +2775,10 @@
         <v>166</v>
       </c>
       <c r="V17" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="W17" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="W17" s="5" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -2834,7 +2823,7 @@
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R18" s="8" t="s">
         <v>190</v>
@@ -2849,10 +2838,10 @@
         <v>166</v>
       </c>
       <c r="V18" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="W18" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="W18" s="5" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
@@ -2862,9 +2851,7 @@
       <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>40</v>
       </c>
@@ -2875,7 +2862,7 @@
         <v>171</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>190</v>
@@ -2887,7 +2874,7 @@
         <v>106</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4" t="s">
@@ -2900,10 +2887,10 @@
         <v>190</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q19" s="8" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="R19" s="8" t="s">
         <v>190</v>
@@ -2921,7 +2908,7 @@
         <v>172</v>
       </c>
       <c r="W19" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -2942,7 +2929,7 @@
         <v>171</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H20" s="25"/>
       <c r="I20" s="3" t="s">
@@ -2952,7 +2939,7 @@
         <v>106</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4" t="s">
@@ -2966,7 +2953,7 @@
       </c>
       <c r="P20" s="8"/>
       <c r="Q20" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="R20" s="8" t="s">
         <v>190</v>
@@ -2984,7 +2971,7 @@
         <v>172</v>
       </c>
       <c r="W20" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -3005,7 +2992,7 @@
         <v>171</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H21" s="25"/>
       <c r="I21" s="3" t="s">
@@ -3015,7 +3002,7 @@
         <v>106</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4" t="s">
@@ -3029,7 +3016,7 @@
       </c>
       <c r="P21" s="8"/>
       <c r="Q21" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="R21" s="8" t="s">
         <v>190</v>
@@ -3047,7 +3034,7 @@
         <v>172</v>
       </c>
       <c r="W21" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -3068,7 +3055,7 @@
         <v>171</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H22" s="25"/>
       <c r="I22" s="3" t="s">
@@ -3125,7 +3112,7 @@
         <v>171</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H23" s="25"/>
       <c r="I23" s="3" t="s">
@@ -3170,7 +3157,7 @@
         <v>171</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H24" s="25"/>
       <c r="I24" s="3" t="s">
@@ -3204,9 +3191,7 @@
       <c r="B25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
         <v>53</v>
       </c>
@@ -3217,7 +3202,7 @@
         <v>171</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>190</v>
@@ -3229,7 +3214,7 @@
         <v>106</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4" t="s">
@@ -3242,10 +3227,10 @@
         <v>190</v>
       </c>
       <c r="P25" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q25" s="8" t="s">
-        <v>334</v>
+        <v>256</v>
       </c>
       <c r="R25" s="8" t="s">
         <v>190</v>
@@ -3260,10 +3245,10 @@
         <v>166</v>
       </c>
       <c r="V25" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="W25" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="W25" s="5" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -3284,7 +3269,7 @@
         <v>171</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="3" t="s">
@@ -3294,7 +3279,7 @@
         <v>106</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4" t="s">
@@ -3308,7 +3293,7 @@
       </c>
       <c r="P26" s="8"/>
       <c r="Q26" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="R26" s="8" t="s">
         <v>190</v>
@@ -3323,10 +3308,10 @@
         <v>166</v>
       </c>
       <c r="V26" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="W26" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="W26" s="5" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -3347,7 +3332,7 @@
         <v>171</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H27" s="26"/>
       <c r="I27" s="3" t="s">
@@ -3357,7 +3342,7 @@
         <v>106</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4" t="s">
@@ -3371,7 +3356,7 @@
       </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="R27" s="8" t="s">
         <v>190</v>
@@ -3386,10 +3371,10 @@
         <v>166</v>
       </c>
       <c r="V27" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="W27" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="W27" s="5" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
@@ -3399,9 +3384,7 @@
       <c r="B28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
         <v>60</v>
       </c>
@@ -3412,7 +3395,7 @@
         <v>171</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>190</v>
@@ -3424,7 +3407,7 @@
         <v>106</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4" t="s">
@@ -3437,10 +3420,10 @@
         <v>190</v>
       </c>
       <c r="P28" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q28" s="8" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="R28" s="8" t="s">
         <v>190</v>
@@ -3458,7 +3441,7 @@
         <v>172</v>
       </c>
       <c r="W28" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -3479,7 +3462,7 @@
         <v>171</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H29" s="25"/>
       <c r="I29" s="3" t="s">
@@ -3489,7 +3472,7 @@
         <v>106</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4" t="s">
@@ -3503,7 +3486,7 @@
       </c>
       <c r="P29" s="8"/>
       <c r="Q29" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R29" s="8" t="s">
         <v>190</v>
@@ -3521,7 +3504,7 @@
         <v>172</v>
       </c>
       <c r="W29" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -3542,7 +3525,7 @@
         <v>171</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H30" s="25"/>
       <c r="I30" s="3" t="s">
@@ -3552,7 +3535,7 @@
         <v>106</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="4" t="s">
@@ -3566,7 +3549,7 @@
       </c>
       <c r="P30" s="8"/>
       <c r="Q30" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R30" s="8" t="s">
         <v>190</v>
@@ -3584,7 +3567,7 @@
         <v>172</v>
       </c>
       <c r="W30" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -3605,7 +3588,7 @@
         <v>171</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H31" s="25"/>
       <c r="I31" s="3" t="s">
@@ -3666,7 +3649,7 @@
         <v>171</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H32" s="25"/>
       <c r="I32" s="3" t="s">
@@ -3729,7 +3712,7 @@
         <v>171</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H33" s="25"/>
       <c r="I33" s="3" t="s">
@@ -3781,9 +3764,7 @@
       <c r="B34" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
         <v>72</v>
       </c>
@@ -3794,7 +3775,7 @@
         <v>171</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>190</v>
@@ -3806,7 +3787,7 @@
         <v>106</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
@@ -3819,10 +3800,10 @@
         <v>190</v>
       </c>
       <c r="P34" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q34" s="8" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="R34" s="8" t="s">
         <v>190</v>
@@ -3837,10 +3818,10 @@
         <v>166</v>
       </c>
       <c r="V34" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="W34" s="5" t="s">
         <v>271</v>
-      </c>
-      <c r="W34" s="5" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -3861,7 +3842,7 @@
         <v>171</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H35" s="25"/>
       <c r="I35" s="3" t="s">
@@ -3871,7 +3852,7 @@
         <v>106</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L35" s="4"/>
       <c r="M35" s="4" t="s">
@@ -3885,7 +3866,7 @@
       </c>
       <c r="P35" s="8"/>
       <c r="Q35" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R35" s="8" t="s">
         <v>190</v>
@@ -3900,10 +3881,10 @@
         <v>166</v>
       </c>
       <c r="V35" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="W35" s="5" t="s">
         <v>271</v>
-      </c>
-      <c r="W35" s="5" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -3924,7 +3905,7 @@
         <v>171</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H36" s="25"/>
       <c r="I36" s="3" t="s">
@@ -3934,7 +3915,7 @@
         <v>106</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4" t="s">
@@ -3948,7 +3929,7 @@
       </c>
       <c r="P36" s="8"/>
       <c r="Q36" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R36" s="8" t="s">
         <v>190</v>
@@ -3963,10 +3944,10 @@
         <v>166</v>
       </c>
       <c r="V36" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="W36" s="5" t="s">
         <v>271</v>
-      </c>
-      <c r="W36" s="5" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -3987,7 +3968,7 @@
         <v>171</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H37" s="25"/>
       <c r="I37" s="3" t="s">
@@ -4032,7 +4013,7 @@
         <v>171</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H38" s="25"/>
       <c r="I38" s="3" t="s">
@@ -4089,7 +4070,7 @@
         <v>171</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H39" s="25"/>
       <c r="I39" s="3" t="s">
@@ -4123,9 +4104,7 @@
       <c r="B40" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
         <v>85</v>
       </c>
@@ -4169,7 +4148,7 @@
         <v>190</v>
       </c>
       <c r="R40" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S40" s="8" t="s">
         <v>190</v>
@@ -4181,10 +4160,10 @@
         <v>166</v>
       </c>
       <c r="V40" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="W40" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.3">
@@ -4194,9 +4173,7 @@
       <c r="B41" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>159</v>
-      </c>
+      <c r="C41" s="16"/>
       <c r="D41" s="16" t="s">
         <v>87</v>
       </c>
@@ -4219,7 +4196,7 @@
         <v>182</v>
       </c>
       <c r="K41" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L41" t="s">
         <v>185</v>
@@ -4240,7 +4217,7 @@
         <v>190</v>
       </c>
       <c r="R41" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S41" s="8" t="s">
         <v>190</v>
@@ -4252,10 +4229,10 @@
         <v>166</v>
       </c>
       <c r="V41" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="W41" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.3">
@@ -4265,9 +4242,7 @@
       <c r="B42" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
         <v>90</v>
       </c>
@@ -4278,7 +4253,7 @@
         <v>171</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H42" s="8" t="s">
         <v>190</v>
@@ -4290,7 +4265,7 @@
         <v>106</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>190</v>
@@ -4305,10 +4280,10 @@
         <v>190</v>
       </c>
       <c r="P42" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q42" s="8" t="s">
-        <v>303</v>
+        <v>256</v>
       </c>
       <c r="R42" s="8" t="s">
         <v>190</v>
@@ -4323,10 +4298,10 @@
         <v>166</v>
       </c>
       <c r="V42" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="W42" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="W42" s="5" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -4347,7 +4322,7 @@
         <v>171</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H43" s="8"/>
       <c r="I43" s="4" t="s">
@@ -4357,7 +4332,7 @@
         <v>106</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L43" s="4" t="s">
         <v>190</v>
@@ -4373,7 +4348,7 @@
       </c>
       <c r="P43" s="8"/>
       <c r="Q43" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="R43" s="8" t="s">
         <v>190</v>
@@ -4388,10 +4363,10 @@
         <v>166</v>
       </c>
       <c r="V43" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="W43" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="W43" s="5" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="44" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -4412,7 +4387,7 @@
         <v>171</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="4" t="s">
@@ -4422,7 +4397,7 @@
         <v>106</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L44" s="4" t="s">
         <v>190</v>
@@ -4438,7 +4413,7 @@
       </c>
       <c r="P44" s="8"/>
       <c r="Q44" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="R44" s="8" t="s">
         <v>190</v>
@@ -4453,10 +4428,10 @@
         <v>166</v>
       </c>
       <c r="V44" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="W44" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="W44" s="5" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -4477,7 +4452,7 @@
         <v>171</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H45" s="8"/>
       <c r="I45" s="4" t="s">
@@ -4487,7 +4462,7 @@
         <v>109</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L45" s="4" t="s">
         <v>190</v>
@@ -4518,10 +4493,10 @@
         <v>166</v>
       </c>
       <c r="V45" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="W45" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="W45" s="5" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="46" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -4542,7 +4517,7 @@
         <v>171</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H46" s="8"/>
       <c r="I46" s="4" t="s">
@@ -4552,7 +4527,7 @@
         <v>109</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L46" s="4" t="s">
         <v>190</v>
@@ -4583,10 +4558,10 @@
         <v>166</v>
       </c>
       <c r="V46" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="W46" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="W46" s="5" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="47" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -4607,7 +4582,7 @@
         <v>171</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H47" s="8"/>
       <c r="I47" s="4" t="s">
@@ -4617,7 +4592,7 @@
         <v>109</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L47" s="4" t="s">
         <v>190</v>
@@ -4648,10 +4623,10 @@
         <v>166</v>
       </c>
       <c r="V47" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="W47" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="W47" s="5" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.3">
@@ -4661,9 +4636,7 @@
       <c r="B48" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C48" s="4"/>
       <c r="D48" s="4" t="s">
         <v>101</v>
       </c>
@@ -4674,7 +4647,7 @@
         <v>171</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>190</v>
@@ -4686,7 +4659,7 @@
         <v>182</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>190</v>
@@ -4707,7 +4680,7 @@
         <v>190</v>
       </c>
       <c r="R48" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="S48" s="8" t="s">
         <v>190</v>
@@ -4719,22 +4692,20 @@
         <v>166</v>
       </c>
       <c r="V48" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="W48" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C49" s="4"/>
       <c r="D49" s="4" t="s">
         <v>104</v>
       </c>
@@ -4745,7 +4716,7 @@
         <v>171</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>190</v>
@@ -4757,7 +4728,7 @@
         <v>182</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>190</v>
@@ -4778,7 +4749,7 @@
         <v>190</v>
       </c>
       <c r="R49" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="S49" s="8" t="s">
         <v>190</v>
@@ -4790,22 +4761,20 @@
         <v>166</v>
       </c>
       <c r="V49" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="W49" s="5" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>188</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>159</v>
-      </c>
+      <c r="C50" s="5"/>
       <c r="D50" s="4" t="s">
         <v>189</v>
       </c>
@@ -4867,16 +4836,14 @@
         <v>190</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>191</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C51" s="4"/>
       <c r="D51" s="4" t="s">
         <v>198</v>
       </c>
@@ -4914,7 +4881,7 @@
         <v>190</v>
       </c>
       <c r="P51" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q51" s="8" t="s">
         <v>208</v>
@@ -4935,19 +4902,17 @@
         <v>172</v>
       </c>
       <c r="W51" s="5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>193</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
         <v>196</v>
       </c>
@@ -4970,7 +4935,7 @@
         <v>109</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>190</v>
@@ -4979,7 +4944,7 @@
         <v>159</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O52" s="8" t="s">
         <v>207</v>
@@ -5006,10 +4971,10 @@
         <v>172</v>
       </c>
       <c r="W52" s="5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>195</v>
       </c>
@@ -5074,16 +5039,14 @@
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>203</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C54" s="4"/>
       <c r="D54" s="4" t="s">
         <v>199</v>
       </c>
@@ -5106,7 +5069,7 @@
         <v>106</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>190</v>
@@ -5121,7 +5084,7 @@
         <v>190</v>
       </c>
       <c r="P54" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q54" s="8" t="s">
         <v>208</v>
@@ -5142,21 +5105,19 @@
         <v>172</v>
       </c>
       <c r="W54" s="5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>205</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C55" s="4"/>
       <c r="D55" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E55" s="17" t="s">
         <v>119</v>
@@ -5177,7 +5138,7 @@
         <v>182</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>190</v>
@@ -5198,7 +5159,7 @@
         <v>190</v>
       </c>
       <c r="R55" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="S55" s="8" t="s">
         <v>190</v>
@@ -5213,10 +5174,10 @@
         <v>172</v>
       </c>
       <c r="W55" s="19" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>210</v>
       </c>
@@ -5261,10 +5222,10 @@
         <v>190</v>
       </c>
       <c r="P56" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q56" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R56" s="8" t="s">
         <v>190</v>
@@ -5279,24 +5240,20 @@
         <v>166</v>
       </c>
       <c r="V56" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="W56" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="W56" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="X56" s="5"/>
-      <c r="Y56" s="5"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>218</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
         <v>230</v>
       </c>
@@ -5319,7 +5276,7 @@
         <v>182</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L57" s="5" t="s">
         <v>190</v>
@@ -5355,12 +5312,10 @@
         <v>172</v>
       </c>
       <c r="W57" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="X57" s="5"/>
-      <c r="Y57" s="5"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>219</v>
       </c>
@@ -5405,13 +5360,13 @@
         <v>190</v>
       </c>
       <c r="P58" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q58" s="8" t="s">
         <v>208</v>
       </c>
       <c r="R58" s="8" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="S58" s="8" t="s">
         <v>174</v>
@@ -5428,19 +5383,15 @@
       <c r="W58" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="X58" s="5"/>
-      <c r="Y58" s="5"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>220</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
         <v>233</v>
       </c>
@@ -5463,7 +5414,7 @@
         <v>182</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L59" s="5" t="s">
         <v>190</v>
@@ -5499,12 +5450,10 @@
         <v>172</v>
       </c>
       <c r="W59" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="X59" s="5"/>
-      <c r="Y59" s="5"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>221</v>
       </c>
@@ -5516,7 +5465,7 @@
         <v>240</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F60" s="8" t="s">
         <v>171</v>
@@ -5525,7 +5474,7 @@
         <v>237</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I60" s="15" t="s">
         <v>105</v>
@@ -5549,10 +5498,10 @@
         <v>190</v>
       </c>
       <c r="P60" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q60" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R60" s="8" t="s">
         <v>190</v>
@@ -5570,12 +5519,10 @@
         <v>172</v>
       </c>
       <c r="W60" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="X60" s="5"/>
-      <c r="Y60" s="5"/>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>222</v>
       </c>
@@ -5587,7 +5534,7 @@
         <v>241</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F61" s="8" t="s">
         <v>171</v>
@@ -5596,7 +5543,7 @@
         <v>238</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I61" s="15" t="s">
         <v>105</v>
@@ -5620,10 +5567,10 @@
         <v>190</v>
       </c>
       <c r="P61" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q61" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R61" s="8" t="s">
         <v>190</v>
@@ -5641,12 +5588,10 @@
         <v>172</v>
       </c>
       <c r="W61" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="X61" s="5"/>
-      <c r="Y61" s="5"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>223</v>
       </c>
@@ -5658,7 +5603,7 @@
         <v>242</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F62" s="8" t="s">
         <v>171</v>
@@ -5667,13 +5612,13 @@
         <v>239</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I62" s="15" t="s">
         <v>105</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K62" s="4" t="s">
         <v>190</v>
@@ -5714,19 +5659,15 @@
       <c r="W62" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="X62" s="5"/>
-      <c r="Y62" s="5"/>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>224</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
         <v>246</v>
       </c>
@@ -5749,7 +5690,7 @@
         <v>106</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>126</v>
+        <v>190</v>
       </c>
       <c r="L63" s="5" t="s">
         <v>190</v>
@@ -5758,19 +5699,19 @@
         <v>159</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>216</v>
+        <v>190</v>
       </c>
       <c r="O63" s="8" t="s">
-        <v>163</v>
+        <v>190</v>
       </c>
       <c r="P63" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q63" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R63" s="8" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="S63" s="8" t="s">
         <v>174</v>
@@ -5785,21 +5726,17 @@
         <v>172</v>
       </c>
       <c r="W63" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="X63" s="5"/>
-      <c r="Y63" s="5"/>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>225</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C64" s="4"/>
       <c r="D64" s="4" t="s">
         <v>249</v>
       </c>
@@ -5819,10 +5756,10 @@
         <v>105</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>126</v>
+        <v>190</v>
       </c>
       <c r="L64" s="5" t="s">
         <v>190</v>
@@ -5837,16 +5774,16 @@
         <v>207</v>
       </c>
       <c r="P64" s="8" t="s">
-        <v>332</v>
+        <v>190</v>
       </c>
       <c r="Q64" s="8" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="R64" s="8" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="S64" s="8" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="T64" s="5" t="s">
         <v>165</v>
@@ -5858,21 +5795,17 @@
         <v>172</v>
       </c>
       <c r="W64" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="X64" s="5"/>
-      <c r="Y64" s="5"/>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>226</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="C65" s="4"/>
       <c r="D65" s="4" t="s">
         <v>247</v>
       </c>
@@ -5910,10 +5843,10 @@
         <v>163</v>
       </c>
       <c r="P65" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q65" s="8" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="R65" s="8" t="s">
         <v>181</v>
@@ -5933,8 +5866,6 @@
       <c r="W65" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="X65" s="5"/>
-      <c r="Y65" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:V65" xr:uid="{5AFA7E03-C988-479B-B08E-B46A33901233}">
@@ -5953,8 +5884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F731B1-F395-44C8-A5FA-27912FB095EB}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5975,7 +5906,7 @@
         <v>151</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -6053,7 +5984,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>127</v>
@@ -6179,7 +6110,7 @@
         <v>209</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>231</v>
@@ -6249,13 +6180,13 @@
         <v>245</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C21" s="24" t="s">
         <v>231</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -6291,7 +6222,7 @@
         <v>235</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>238</v>
@@ -6305,7 +6236,7 @@
         <v>236</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C25" s="24" t="s">
         <v>239</v>
@@ -6325,7 +6256,7 @@
         <v>237</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>252</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>